<commit_message>
Implement test cases for Project Page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Login.xlsx
+++ b/src/test/resources/testData/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>email</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Testing 02</t>
+  </si>
+  <si>
+    <t>error message</t>
+  </si>
+  <si>
+    <t>Missing required parameter USERNAME</t>
+  </si>
+  <si>
+    <t>Incorrect username or password.</t>
   </si>
 </sst>
 </file>
@@ -103,9 +112,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -387,56 +399,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
@@ -450,6 +482,7 @@
     <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -457,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>